<commit_message>
Add Text File [practice_7_29.xlsx]
</commit_message>
<xml_diff>
--- a/practice_7_29.xlsx
+++ b/practice_7_29.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Education\speed_typing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김지혁\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D451B03-8BE0-4716-B905-EEF3C5693B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B31CF4A-EB30-42F9-AB31-5CF037D1894B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="975" windowWidth="16935" windowHeight="13680" xr2:uid="{113D0C04-CC4B-4748-B481-962982009824}"/>
+    <workbookView xWindow="540" yWindow="975" windowWidth="17010" windowHeight="13680" xr2:uid="{113D0C04-CC4B-4748-B481-962982009824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
   <si>
     <t>자리연습</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -314,6 +314,34 @@
   </si>
   <si>
     <t>7월 29일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2분 24초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3분 7초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3분 8초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3분 17초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3분 22초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">짧은글 연습 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>302타 98%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -324,7 +352,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +363,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -510,7 +546,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -590,6 +626,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -906,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28C4D32-81F1-4D5F-928A-FA061A784D7C}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1183,7 +1222,9 @@
       <c r="I12" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="8"/>
+      <c r="J12" s="24" t="s">
+        <v>72</v>
+      </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
@@ -1210,7 +1251,9 @@
       <c r="I13" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="8"/>
+      <c r="J13" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
@@ -1237,7 +1280,9 @@
       <c r="I14" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="J14" s="8"/>
+      <c r="J14" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -1264,7 +1309,9 @@
       <c r="I15" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="8"/>
+      <c r="J15" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -1291,14 +1338,16 @@
       <c r="I16" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="8"/>
+      <c r="J16" s="24" t="s">
+        <v>74</v>
+      </c>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C17" s="18" t="s">
         <v>7</v>
       </c>
@@ -1318,14 +1367,16 @@
       <c r="I17" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="J17" s="8"/>
+      <c r="J17" s="24" t="s">
+        <v>75</v>
+      </c>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C18" s="18" t="s">
         <v>8</v>
       </c>
@@ -1345,14 +1396,16 @@
       <c r="I18" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="J18" s="24" t="s">
+        <v>76</v>
+      </c>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="9"/>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C19" s="19" t="s">
         <v>9</v>
       </c>
@@ -1372,13 +1425,23 @@
       <c r="I19" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="J19" s="12"/>
+      <c r="J19" s="26" t="s">
+        <v>50</v>
+      </c>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
       <c r="O19" s="13"/>
     </row>
+    <row r="20" spans="2:15" s="27" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="B20" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>